<commit_message>
added fairness and test vs lockdown plots and data files
</commit_message>
<xml_diff>
--- a/benchmarks/results/plots/results-Fig1.xlsx
+++ b/benchmarks/results/plots/results-Fig1.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H533"/>
+  <dimension ref="A1:H541"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15368,6 +15368,230 @@
         <v>-3.309322252153853e+23</v>
       </c>
     </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=age_group_gradient_targetGroups=True_targetAct=False_targetTests=False</t>
+        </is>
+      </c>
+      <c r="B534" t="n">
+        <v>50</v>
+      </c>
+      <c r="C534" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D534" t="n">
+        <v>60000</v>
+      </c>
+      <c r="E534" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F534" t="n">
+        <v>52.97564769386039</v>
+      </c>
+      <c r="G534" t="n">
+        <v>1868.070516240173</v>
+      </c>
+      <c r="H534" t="n">
+        <v>49501127135.07371</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=age_group_gradient_targetGroups=True_targetAct=False_targetTests=False</t>
+        </is>
+      </c>
+      <c r="B535" t="n">
+        <v>50</v>
+      </c>
+      <c r="C535" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D535" t="n">
+        <v>120000</v>
+      </c>
+      <c r="E535" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F535" t="n">
+        <v>53.06393615750851</v>
+      </c>
+      <c r="G535" t="n">
+        <v>1821.193960486289</v>
+      </c>
+      <c r="H535" t="n">
+        <v>49676603718.91109</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=age_group_gradient_targetGroups=True_targetAct=False_targetTests=False</t>
+        </is>
+      </c>
+      <c r="B536" t="n">
+        <v>50</v>
+      </c>
+      <c r="C536" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D536" t="n">
+        <v>240000</v>
+      </c>
+      <c r="E536" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F536" t="n">
+        <v>52.69334229288796</v>
+      </c>
+      <c r="G536" t="n">
+        <v>1426.416571816286</v>
+      </c>
+      <c r="H536" t="n">
+        <v>50040276650.5134</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=age_group_gradient_targetGroups=True_targetAct=False_targetTests=False</t>
+        </is>
+      </c>
+      <c r="B537" t="n">
+        <v>50</v>
+      </c>
+      <c r="C537" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D537" t="n">
+        <v>360000</v>
+      </c>
+      <c r="E537" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F537" t="n">
+        <v>52.70093459161686</v>
+      </c>
+      <c r="G537" t="n">
+        <v>1801.951147482135</v>
+      </c>
+      <c r="H537" t="n">
+        <v>49349392851.93075</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=age_group_gradient_targetGroups=True_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B538" t="n">
+        <v>50</v>
+      </c>
+      <c r="C538" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D538" t="n">
+        <v>60000</v>
+      </c>
+      <c r="E538" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F538" t="n">
+        <v>52.98238601317134</v>
+      </c>
+      <c r="G538" t="n">
+        <v>1776.946010866787</v>
+      </c>
+      <c r="H538" t="n">
+        <v>49677352614.84064</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=age_group_gradient_targetGroups=True_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B539" t="n">
+        <v>50</v>
+      </c>
+      <c r="C539" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D539" t="n">
+        <v>120000</v>
+      </c>
+      <c r="E539" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F539" t="n">
+        <v>53.07388983985473</v>
+      </c>
+      <c r="G539" t="n">
+        <v>1680.452738282573</v>
+      </c>
+      <c r="H539" t="n">
+        <v>49948329248.60695</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=age_group_gradient_targetGroups=True_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B540" t="n">
+        <v>50</v>
+      </c>
+      <c r="C540" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D540" t="n">
+        <v>240000</v>
+      </c>
+      <c r="E540" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F540" t="n">
+        <v>52.97304648324432</v>
+      </c>
+      <c r="G540" t="n">
+        <v>1411.228643471699</v>
+      </c>
+      <c r="H540" t="n">
+        <v>50348229650.97617</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>linearization_heuristic_optBouncing=False_initial_uhat=age_group_gradient_targetGroups=True_targetAct=False_targetTests=True</t>
+        </is>
+      </c>
+      <c r="B541" t="n">
+        <v>50</v>
+      </c>
+      <c r="C541" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D541" t="n">
+        <v>360000</v>
+      </c>
+      <c r="E541" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F541" t="n">
+        <v>52.71130665491413</v>
+      </c>
+      <c r="G541" t="n">
+        <v>1579.370988188422</v>
+      </c>
+      <c r="H541" t="n">
+        <v>49773753216.37659</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>